<commit_message>
Alpha Diversity - Eve
</commit_message>
<xml_diff>
--- a/results/DFs/DF_AlphaDiversity.xlsx
+++ b/results/DFs/DF_AlphaDiversity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliana/Documents/GitHub/SMS-6198-22-ITS/results/DFs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CD6F63-9921-3A4F-A8C4-1E3336341809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB839A9-3D5F-014F-B173-F62E7F0A8686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="1580" windowWidth="28860" windowHeight="14480" activeTab="1" xr2:uid="{417D1A7B-12E1-2449-9433-679CEA003D64}"/>
+    <workbookView xWindow="4600" yWindow="3080" windowWidth="33240" windowHeight="18540" activeTab="2" xr2:uid="{417D1A7B-12E1-2449-9433-679CEA003D64}"/>
   </bookViews>
   <sheets>
     <sheet name="Full_Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="DF_Main_Data" localSheetId="1">Main_Data!$A$1:$U$46</definedName>
     <definedName name="DF_Main_Data_ACE" localSheetId="2">Merged_Main_Data!$A$1:$B$16</definedName>
     <definedName name="DF_Main_Data_Chao1" localSheetId="2">Merged_Main_Data!#REF!</definedName>
-    <definedName name="DF_Main_Data_Eveness" localSheetId="1">Main_Data!$J$1:$J$46</definedName>
+    <definedName name="DF_Main_Data_Eveness" localSheetId="1">Main_Data!#REF!</definedName>
     <definedName name="DF_Main_Data_Fisher" localSheetId="2">Merged_Main_Data!#REF!</definedName>
     <definedName name="DF_Main_Data_InvSimpson" localSheetId="2">Merged_Main_Data!#REF!</definedName>
     <definedName name="DF_Main_Data_Observed" localSheetId="2">Merged_Main_Data!#REF!</definedName>
@@ -30,6 +30,7 @@
     <definedName name="DF_Main_Data_se.chao1" localSheetId="2">Merged_Main_Data!#REF!</definedName>
     <definedName name="DF_Main_Data_Shannon" localSheetId="2">Merged_Main_Data!#REF!</definedName>
     <definedName name="DF_Main_Data_Simpson" localSheetId="2">Merged_Main_Data!$L$1:$L$16</definedName>
+    <definedName name="ExternalData_1" localSheetId="1">Main_Data!$J$1:$J$46</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -106,8 +107,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{87CC20CC-720C-C445-A717-37E9344DCBC6}" name="DF_Main_Data_Eveness" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/juliana/Documents/GitHub/SMS-6198-22-ITS/results/DFs/DF_Main_Data_Eveness.tsv" decimal="," thousands=".">
+  <connection id="4" xr16:uid="{F9C25875-F33B-6640-958E-BF4F26623047}" name="DF_Main_Data_Eveness1" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/juliana/Documents/GitHub/SMS-6198-22-ITS/results/DF_Main_Data_Eveness.tsv" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="418">
   <si>
     <t>Observed</t>
   </si>
@@ -1245,6 +1246,141 @@
   </si>
   <si>
     <t>Evenness</t>
+  </si>
+  <si>
+    <t>0.527738813869171</t>
+  </si>
+  <si>
+    <t>0.428118253994628</t>
+  </si>
+  <si>
+    <t>0.560619047034596</t>
+  </si>
+  <si>
+    <t>0.636402551537277</t>
+  </si>
+  <si>
+    <t>0.673721732710049</t>
+  </si>
+  <si>
+    <t>0.382665220890061</t>
+  </si>
+  <si>
+    <t>0.535339425192582</t>
+  </si>
+  <si>
+    <t>0.684987394860404</t>
+  </si>
+  <si>
+    <t>0.380717672289544</t>
+  </si>
+  <si>
+    <t>0.344054285958952</t>
+  </si>
+  <si>
+    <t>0.468125365354258</t>
+  </si>
+  <si>
+    <t>0.621941665309819</t>
+  </si>
+  <si>
+    <t>0.655496333274333</t>
+  </si>
+  <si>
+    <t>0.259103008887306</t>
+  </si>
+  <si>
+    <t>0.423371636914216</t>
+  </si>
+  <si>
+    <t>0.728329596326734</t>
+  </si>
+  <si>
+    <t>0.713910278465967</t>
+  </si>
+  <si>
+    <t>0.603234451585657</t>
+  </si>
+  <si>
+    <t>0.441380686996997</t>
+  </si>
+  <si>
+    <t>0.687594352662858</t>
+  </si>
+  <si>
+    <t>0.69937980088338</t>
+  </si>
+  <si>
+    <t>0.63775675860197</t>
+  </si>
+  <si>
+    <t>0.542078829850437</t>
+  </si>
+  <si>
+    <t>0.572567507470407</t>
+  </si>
+  <si>
+    <t>0.637441988153252</t>
+  </si>
+  <si>
+    <t>0.584605694469264</t>
+  </si>
+  <si>
+    <t>0.69707793837814</t>
+  </si>
+  <si>
+    <t>0.528788280240409</t>
+  </si>
+  <si>
+    <t>0.5928153821021</t>
+  </si>
+  <si>
+    <t>0.40577467809636</t>
+  </si>
+  <si>
+    <t>0.619070629174783</t>
+  </si>
+  <si>
+    <t>0.677039327279401</t>
+  </si>
+  <si>
+    <t>0.674719492886561</t>
+  </si>
+  <si>
+    <t>0.646014898713823</t>
+  </si>
+  <si>
+    <t>0.721976687506446</t>
+  </si>
+  <si>
+    <t>0.667985166433732</t>
+  </si>
+  <si>
+    <t>0.651770433075049</t>
+  </si>
+  <si>
+    <t>0.68085941813833</t>
+  </si>
+  <si>
+    <t>0.60738819473163</t>
+  </si>
+  <si>
+    <t>0.6094150915864</t>
+  </si>
+  <si>
+    <t>0.635136098432655</t>
+  </si>
+  <si>
+    <t>0.673067309672451</t>
+  </si>
+  <si>
+    <t>0.60546742856538</t>
+  </si>
+  <si>
+    <t>0.56744395071217</t>
+  </si>
+  <si>
+    <t>0.627557698438315</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1441,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DF_Main_Data_Eveness" connectionId="4" xr16:uid="{EF77B255-B6F4-1F47-B0F3-9FE3B754C7E2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="4" xr16:uid="{CCABA4AA-B052-CF4F-BAEA-AD5E45D0DA24}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5258,8 +5394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{400FBBB9-6519-5040-AB9D-5D4729D1E2FA}">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5271,7 +5407,7 @@
     <col min="5" max="6" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -5379,8 +5515,8 @@
       <c r="I2" s="1">
         <v>297328908078602</v>
       </c>
-      <c r="J2" s="1">
-        <v>548063892334199</v>
+      <c r="J2" t="s">
+        <v>373</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>13</v>
@@ -5444,8 +5580,8 @@
       <c r="I3" s="1">
         <v>152169732202265</v>
       </c>
-      <c r="J3" s="1">
-        <v>489783979995091</v>
+      <c r="J3" t="s">
+        <v>374</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>19</v>
@@ -5509,8 +5645,8 @@
       <c r="I4" s="1">
         <v>243336073202731</v>
       </c>
-      <c r="J4" s="1">
-        <v>531320597904179</v>
+      <c r="J4" t="s">
+        <v>375</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>23</v>
@@ -5574,8 +5710,8 @@
       <c r="I5" s="1">
         <v>402269050556998</v>
       </c>
-      <c r="J5" s="1">
-        <v>569035945432406</v>
+      <c r="J5" t="s">
+        <v>376</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>27</v>
@@ -5639,8 +5775,8 @@
       <c r="I6" s="1">
         <v>443224541912522</v>
       </c>
-      <c r="J6" s="1">
-        <v>576205138278018</v>
+      <c r="J6" t="s">
+        <v>377</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>39</v>
@@ -5704,8 +5840,8 @@
       <c r="I7" s="1">
         <v>120591249586571</v>
       </c>
-      <c r="J7" s="1">
-        <v>466343909411207</v>
+      <c r="J7" t="s">
+        <v>378</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>42</v>
@@ -5769,8 +5905,8 @@
       <c r="I8" s="1">
         <v>275365319442134</v>
       </c>
-      <c r="J8" s="1">
-        <v>541164605185504</v>
+      <c r="J8" t="s">
+        <v>379</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>45</v>
@@ -5834,8 +5970,8 @@
       <c r="I9" s="1">
         <v>415721697071872</v>
       </c>
-      <c r="J9" s="1">
-        <v>569035945432406</v>
+      <c r="J9" t="s">
+        <v>380</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>47</v>
@@ -5899,8 +6035,8 @@
       <c r="I10" s="1">
         <v>252736475986516</v>
       </c>
-      <c r="J10" s="1">
-        <v>536129216570943</v>
+      <c r="J10" t="s">
+        <v>381</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>57</v>
@@ -5964,8 +6100,8 @@
       <c r="I11" s="1">
         <v>158109402948741</v>
       </c>
-      <c r="J11" s="1">
-        <v>489034912822175</v>
+      <c r="J11" t="s">
+        <v>382</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>59</v>
@@ -6029,8 +6165,8 @@
       <c r="I12" s="1">
         <v>230982047263278</v>
       </c>
-      <c r="J12" s="1">
-        <v>52040066870768</v>
+      <c r="J12" t="s">
+        <v>383</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>62</v>
@@ -6094,8 +6230,8 @@
       <c r="I13" s="1">
         <v>493519301522078</v>
       </c>
-      <c r="J13" s="1">
-        <v>584643877505772</v>
+      <c r="J13" t="s">
+        <v>384</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>64</v>
@@ -6159,8 +6295,8 @@
       <c r="I14" s="1">
         <v>514838493479089</v>
       </c>
-      <c r="J14" s="1">
-        <v>590808293816893</v>
+      <c r="J14" t="s">
+        <v>385</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>76</v>
@@ -6224,8 +6360,8 @@
       <c r="I15" s="1">
         <v>217805315893001</v>
       </c>
-      <c r="J15" s="1">
-        <v>523110861685459</v>
+      <c r="J15" t="s">
+        <v>386</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>80</v>
@@ -6289,8 +6425,8 @@
       <c r="I16" s="1">
         <v>182880499433165</v>
       </c>
-      <c r="J16" s="1">
-        <v>507517381523383</v>
+      <c r="J16" t="s">
+        <v>387</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>83</v>
@@ -6354,8 +6490,8 @@
       <c r="I17" s="1">
         <v>358865320040781</v>
       </c>
-      <c r="J17" s="1">
-        <v>545958551414416</v>
+      <c r="J17" t="s">
+        <v>388</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>85</v>
@@ -6419,8 +6555,8 @@
       <c r="I18" s="1">
         <v>631918340345687</v>
       </c>
-      <c r="J18" s="1">
-        <v>607764224334903</v>
+      <c r="J18" t="s">
+        <v>389</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>96</v>
@@ -6484,8 +6620,8 @@
       <c r="I19" s="1">
         <v>353919735196274</v>
       </c>
-      <c r="J19" s="1">
-        <v>560947179518496</v>
+      <c r="J19" t="s">
+        <v>390</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>99</v>
@@ -6549,8 +6685,8 @@
       <c r="I20" s="1">
         <v>246785720388643</v>
       </c>
-      <c r="J20" s="1">
-        <v>532787616878958</v>
+      <c r="J20" t="s">
+        <v>391</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>102</v>
@@ -6614,8 +6750,8 @@
       <c r="I21" s="1">
         <v>329849846387107</v>
       </c>
-      <c r="J21" s="1">
-        <v>546806014113513</v>
+      <c r="J21" t="s">
+        <v>392</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>104</v>
@@ -6679,8 +6815,8 @@
       <c r="I22" s="1">
         <v>602527871562293</v>
       </c>
-      <c r="J22" s="1">
-        <v>605443934626937</v>
+      <c r="J22" t="s">
+        <v>393</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>114</v>
@@ -6744,8 +6880,8 @@
       <c r="I23" s="1">
         <v>313512291135976</v>
       </c>
-      <c r="J23" s="1">
-        <v>54249500174814</v>
+      <c r="J23" t="s">
+        <v>394</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>116</v>
@@ -6809,8 +6945,8 @@
       <c r="I24" s="1">
         <v>207895330362197</v>
       </c>
-      <c r="J24" s="1">
-        <v>50998664278242</v>
+      <c r="J24" t="s">
+        <v>395</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>118</v>
@@ -6874,8 +7010,8 @@
       <c r="I25" s="1">
         <v>284142669685876</v>
       </c>
-      <c r="J25" s="1">
-        <v>537527840768417</v>
+      <c r="J25" t="s">
+        <v>396</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>120</v>
@@ -6939,8 +7075,8 @@
       <c r="I26" s="1">
         <v>201774607271233</v>
       </c>
-      <c r="J26" s="1">
-        <v>503695260241363</v>
+      <c r="J26" t="s">
+        <v>397</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>130</v>
@@ -7004,8 +7140,8 @@
       <c r="I27" s="1">
         <v>448816163981768</v>
       </c>
-      <c r="J27" s="1">
-        <v>575257263882563</v>
+      <c r="J27" t="s">
+        <v>398</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>132</v>
@@ -7069,8 +7205,8 @@
       <c r="I28" s="1">
         <v>339946084241505</v>
       </c>
-      <c r="J28" s="1">
-        <v>54971682252932</v>
+      <c r="J28" t="s">
+        <v>399</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>134</v>
@@ -7134,8 +7270,8 @@
       <c r="I29" s="1">
         <v>219793111711595</v>
       </c>
-      <c r="J29" s="1">
-        <v>512396397940326</v>
+      <c r="J29" t="s">
+        <v>400</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>136</v>
@@ -7199,8 +7335,8 @@
       <c r="I30" s="1">
         <v>522591537237823</v>
       </c>
-      <c r="J30" s="1">
-        <v>592958914338989</v>
+      <c r="J30" t="s">
+        <v>401</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>148</v>
@@ -7264,8 +7400,8 @@
       <c r="I31" s="1">
         <v>282958730394217</v>
       </c>
-      <c r="J31" s="1">
-        <v>54510384535657</v>
+      <c r="J31" t="s">
+        <v>402</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>150</v>
@@ -7329,8 +7465,8 @@
       <c r="I32" s="1">
         <v>254230926801996</v>
       </c>
-      <c r="J32" s="1">
-        <v>527811465923052</v>
+      <c r="J32" t="s">
+        <v>403</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>152</v>
@@ -7394,8 +7530,8 @@
       <c r="I33" s="1">
         <v>401161581156067</v>
       </c>
-      <c r="J33" s="1">
-        <v>568357976733868</v>
+      <c r="J33" t="s">
+        <v>404</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>154</v>
@@ -7459,8 +7595,8 @@
       <c r="I34" s="1">
         <v>394902669391261</v>
       </c>
-      <c r="J34" s="1">
-        <v>565599181081985</v>
+      <c r="J34" t="s">
+        <v>405</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>164</v>
@@ -7524,8 +7660,8 @@
       <c r="I35" s="1">
         <v>468055329782063</v>
       </c>
-      <c r="J35" s="1">
-        <v>578996017089725</v>
+      <c r="J35" t="s">
+        <v>406</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>167</v>
@@ -7589,8 +7725,8 @@
       <c r="I36" s="1">
         <v>351143150583439</v>
       </c>
-      <c r="J36" s="1">
-        <v>552146091786225</v>
+      <c r="J36" t="s">
+        <v>407</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>169</v>
@@ -7654,8 +7790,8 @@
       <c r="I37" s="1">
         <v>263937975750735</v>
       </c>
-      <c r="J37" s="1">
-        <v>533271879326537</v>
+      <c r="J37" t="s">
+        <v>408</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>171</v>
@@ -7719,8 +7855,8 @@
       <c r="I38" s="1">
         <v>271780332591292</v>
       </c>
-      <c r="J38" s="1">
-        <v>527299955856375</v>
+      <c r="J38" t="s">
+        <v>409</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>181</v>
@@ -7784,8 +7920,8 @@
       <c r="I39" s="1">
         <v>411607969527042</v>
       </c>
-      <c r="J39" s="1">
-        <v>563835466933375</v>
+      <c r="J39" t="s">
+        <v>410</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>184</v>
@@ -7849,8 +7985,8 @@
       <c r="I40" s="1">
         <v>333993757919604</v>
       </c>
-      <c r="J40" s="1">
-        <v>549306144334055</v>
+      <c r="J40" t="s">
+        <v>411</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>187</v>
@@ -7914,8 +8050,8 @@
       <c r="I41" s="1">
         <v>189356966204034</v>
       </c>
-      <c r="J41" s="1">
-        <v>493447393313069</v>
+      <c r="J41" t="s">
+        <v>412</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>196</v>
@@ -7979,8 +8115,8 @@
       <c r="I42" s="1">
         <v>392786987428135</v>
       </c>
-      <c r="J42" s="1">
-        <v>556452040732269</v>
+      <c r="J42" t="s">
+        <v>413</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>198</v>
@@ -8044,8 +8180,8 @@
       <c r="I43" s="1">
         <v>450806862607642</v>
       </c>
-      <c r="J43" s="1">
-        <v>570044357339069</v>
+      <c r="J43" t="s">
+        <v>414</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>201</v>
@@ -8109,8 +8245,8 @@
       <c r="I44" s="1">
         <v>222799044714598</v>
       </c>
-      <c r="J44" s="1">
-        <v>508759633523238</v>
+      <c r="J44" t="s">
+        <v>415</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>211</v>
@@ -8174,8 +8310,8 @@
       <c r="I45" s="1">
         <v>337153715796528</v>
       </c>
-      <c r="J45" s="1">
-        <v>546806014113513</v>
+      <c r="J45" t="s">
+        <v>416</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>213</v>
@@ -8239,8 +8375,8 @@
       <c r="I46" s="1">
         <v>388430086221479</v>
       </c>
-      <c r="J46" s="1">
-        <v>557972982598622</v>
+      <c r="J46" t="s">
+        <v>417</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>215</v>
@@ -8285,7 +8421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA554EE7-C051-C349-ABED-8E1A9A6027AC}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>

</xml_diff>